<commit_message>
Sync up base.yaml with WC Ports LCOE analsyis
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
         <v>2030</v>
       </c>
       <c r="B2" t="n">
-        <v>515.8347223440652</v>
+        <v>403.8461538461539</v>
       </c>
     </row>
     <row r="3">
@@ -461,7 +461,7 @@
         <v>2031</v>
       </c>
       <c r="B3" t="n">
-        <v>1284.348131251097</v>
+        <v>1005.564443207901</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         <v>2032</v>
       </c>
       <c r="B4" t="n">
-        <v>2568.738740592881</v>
+        <v>2033.048913453275</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         <v>2033</v>
       </c>
       <c r="B5" t="n">
-        <v>4110.019301631865</v>
+        <v>3265.929493563985</v>
       </c>
     </row>
     <row r="6">
@@ -485,7 +485,7 @@
         <v>2034</v>
       </c>
       <c r="B6" t="n">
-        <v>5647.131075627302</v>
+        <v>4490.929259706946</v>
       </c>
     </row>
     <row r="7">
@@ -493,7 +493,7 @@
         <v>2035</v>
       </c>
       <c r="B7" t="n">
-        <v>7184.242849622741</v>
+        <v>5721.18277145531</v>
       </c>
     </row>
     <row r="8">
@@ -501,7 +501,7 @@
         <v>2036</v>
       </c>
       <c r="B8" t="n">
-        <v>8919.31785782061</v>
+        <v>6952.975212518215</v>
       </c>
     </row>
     <row r="9">
@@ -509,7 +509,7 @@
         <v>2037</v>
       </c>
       <c r="B9" t="n">
-        <v>10718.24237129987</v>
+        <v>8361.529460239752</v>
       </c>
     </row>
     <row r="10">
@@ -517,7 +517,7 @@
         <v>2038</v>
       </c>
       <c r="B10" t="n">
-        <v>12512.21163574988</v>
+        <v>9798.398227727481</v>
       </c>
     </row>
     <row r="11">
@@ -525,7 +525,7 @@
         <v>2039</v>
       </c>
       <c r="B11" t="n">
-        <v>14306.27019762059</v>
+        <v>11239.83113733724</v>
       </c>
     </row>
     <row r="12">
@@ -533,7 +533,7 @@
         <v>2040</v>
       </c>
       <c r="B12" t="n">
-        <v>16169.04706157809</v>
+        <v>12675.55655747152</v>
       </c>
     </row>
     <row r="13">
@@ -541,7 +541,7 @@
         <v>2041</v>
       </c>
       <c r="B13" t="n">
-        <v>18217.07312091846</v>
+        <v>14113.92646310739</v>
       </c>
     </row>
     <row r="14">
@@ -549,7 +549,7 @@
         <v>2042</v>
       </c>
       <c r="B14" t="n">
-        <v>20247.36595645048</v>
+        <v>15555.53703237736</v>
       </c>
     </row>
     <row r="15">
@@ -557,7 +557,7 @@
         <v>2043</v>
       </c>
       <c r="B15" t="n">
-        <v>21324.16295949426</v>
+        <v>17092.33012812059</v>
       </c>
     </row>
     <row r="16">
@@ -565,7 +565,7 @@
         <v>2044</v>
       </c>
       <c r="B16" t="n">
-        <v>22339.70203571022</v>
+        <v>18735.76715941676</v>
       </c>
     </row>
     <row r="17">
@@ -573,7 +573,7 @@
         <v>2045</v>
       </c>
       <c r="B17" t="n">
-        <v>23348.58948847009</v>
+        <v>19997.24720132134</v>
       </c>
     </row>
     <row r="18">
@@ -581,7 +581,7 @@
         <v>2046</v>
       </c>
       <c r="B18" t="n">
-        <v>24374.03418403184</v>
+        <v>20811.18751161494</v>
       </c>
     </row>
     <row r="19">
@@ -589,7 +589,7 @@
         <v>2047</v>
       </c>
       <c r="B19" t="n">
-        <v>25388.14966450586</v>
+        <v>21625.10452476075</v>
       </c>
     </row>
     <row r="20">
@@ -597,7 +597,7 @@
         <v>2048</v>
       </c>
       <c r="B20" t="n">
-        <v>26395.69187543901</v>
+        <v>22433.56579188842</v>
       </c>
     </row>
     <row r="21">
@@ -605,7 +605,7 @@
         <v>2049</v>
       </c>
       <c r="B21" t="n">
-        <v>27424.02247717162</v>
+        <v>23242.59035584874</v>
       </c>
     </row>
     <row r="22">
@@ -613,7 +613,7 @@
         <v>2050</v>
       </c>
       <c r="B22" t="n">
-        <v>28436.71102012965</v>
+        <v>24056.49507526482</v>
       </c>
     </row>
     <row r="23">
@@ -621,7 +621,7 @@
         <v>2051</v>
       </c>
       <c r="B23" t="n">
-        <v>29445.68016857879</v>
+        <v>24870.47017283033</v>
       </c>
     </row>
     <row r="24">
@@ -629,7 +629,7 @@
         <v>2052</v>
       </c>
       <c r="B24" t="n">
-        <v>30471.20112385858</v>
+        <v>25675.90383556616</v>
       </c>
     </row>
     <row r="25">
@@ -637,7 +637,7 @@
         <v>2053</v>
       </c>
       <c r="B25" t="n">
-        <v>31485.27237575344</v>
+        <v>26487.96803865094</v>
       </c>
     </row>
     <row r="26">
@@ -645,7 +645,7 @@
         <v>2054</v>
       </c>
       <c r="B26" t="n">
-        <v>32495.61044129697</v>
+        <v>27301.89555844638</v>
       </c>
     </row>
     <row r="27">
@@ -653,7 +653,7 @@
         <v>2055</v>
       </c>
       <c r="B27" t="n">
-        <v>33521.07234839616</v>
+        <v>28114.42466507616</v>
       </c>
     </row>
     <row r="28">
@@ -661,7 +661,63 @@
         <v>2056</v>
       </c>
       <c r="B28" t="n">
-        <v>34546.59330367595</v>
+        <v>28918.2418792439</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B29" t="n">
+        <v>29733.34572145313</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B30" t="n">
+        <v>30547.29604162795</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B31" t="n">
+        <v>31356.72997522708</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B32" t="n">
+        <v>32162.51626091804</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2061</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32978.721427244</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2062</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33792.6228746632</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2063</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34606.57870284334</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +731,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,7 +756,7 @@
         <v>2030</v>
       </c>
       <c r="B2" t="n">
-        <v>515.8347223440652</v>
+        <v>408.9581304771178</v>
       </c>
     </row>
     <row r="3">
@@ -708,7 +764,7 @@
         <v>2031</v>
       </c>
       <c r="B3" t="n">
-        <v>1284.348131251097</v>
+        <v>1018.223551505877</v>
       </c>
     </row>
     <row r="4">
@@ -716,7 +772,7 @@
         <v>2032</v>
       </c>
       <c r="B4" t="n">
-        <v>2515.834722344065</v>
+        <v>2045.708021751251</v>
       </c>
     </row>
     <row r="5">
@@ -724,7 +780,7 @@
         <v>2033</v>
       </c>
       <c r="B5" t="n">
-        <v>4572.882397908923</v>
+        <v>3884.708584548976</v>
       </c>
     </row>
     <row r="6">
@@ -732,7 +788,7 @@
         <v>2034</v>
       </c>
       <c r="B6" t="n">
-        <v>6878.487453939287</v>
+        <v>5718.98763398018</v>
       </c>
     </row>
     <row r="7">
@@ -740,7 +796,7 @@
         <v>2035</v>
       </c>
       <c r="B7" t="n">
-        <v>9201.843463810765</v>
+        <v>7553.149796348535</v>
       </c>
     </row>
     <row r="8">
@@ -748,7 +804,7 @@
         <v>2036</v>
       </c>
       <c r="B8" t="n">
-        <v>11962.45076452843</v>
+        <v>9409.450157970316</v>
       </c>
     </row>
     <row r="9">
@@ -756,7 +812,7 @@
         <v>2037</v>
       </c>
       <c r="B9" t="n">
-        <v>14789.7734875585</v>
+        <v>11634.13373766249</v>
       </c>
     </row>
     <row r="10">
@@ -764,7 +820,7 @@
         <v>2038</v>
       </c>
       <c r="B10" t="n">
-        <v>17815.03233480562</v>
+        <v>13881.85941608445</v>
       </c>
     </row>
     <row r="11">
@@ -772,7 +828,7 @@
         <v>2039</v>
       </c>
       <c r="B11" t="n">
-        <v>20891.3782886815</v>
+        <v>16201.89501145963</v>
       </c>
     </row>
     <row r="12">
@@ -780,7 +836,7 @@
         <v>2040</v>
       </c>
       <c r="B12" t="n">
-        <v>23967.92320299695</v>
+        <v>18651.91618999467</v>
       </c>
     </row>
     <row r="13">
@@ -788,7 +844,7 @@
         <v>2041</v>
       </c>
       <c r="B13" t="n">
-        <v>26840.70612470093</v>
+        <v>21108.29106167314</v>
       </c>
     </row>
     <row r="14">
@@ -796,7 +852,7 @@
         <v>2042</v>
       </c>
       <c r="B14" t="n">
-        <v>29203.46523062515</v>
+        <v>23558.38741141113</v>
       </c>
     </row>
     <row r="15">
@@ -804,7 +860,7 @@
         <v>2043</v>
       </c>
       <c r="B15" t="n">
-        <v>30968.54503830431</v>
+        <v>26008.09314700343</v>
       </c>
     </row>
     <row r="16">
@@ -812,7 +868,7 @@
         <v>2044</v>
       </c>
       <c r="B16" t="n">
-        <v>32305.7473955285</v>
+        <v>28457.75669533716</v>
       </c>
     </row>
     <row r="17">
@@ -820,7 +876,7 @@
         <v>2045</v>
       </c>
       <c r="B17" t="n">
-        <v>33333.99672207914</v>
+        <v>30420.8863699712</v>
       </c>
     </row>
     <row r="18">
@@ -828,7 +884,39 @@
         <v>2046</v>
       </c>
       <c r="B18" t="n">
-        <v>34359.51767735893</v>
+        <v>31234.80765656941</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B19" t="n">
+        <v>32048.7782216854</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B20" t="n">
+        <v>32862.67769209328</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B21" t="n">
+        <v>33678.87009849471</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B22" t="n">
+        <v>34492.79940537025</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -867,7 +955,7 @@
         <v>2030</v>
       </c>
       <c r="B2" t="n">
-        <v>515.8347223440652</v>
+        <v>408.9581304771178</v>
       </c>
     </row>
     <row r="3">
@@ -875,7 +963,7 @@
         <v>2031</v>
       </c>
       <c r="B3" t="n">
-        <v>1284.348131251097</v>
+        <v>1018.223551505877</v>
       </c>
     </row>
     <row r="4">
@@ -883,7 +971,7 @@
         <v>2032</v>
       </c>
       <c r="B4" t="n">
-        <v>2515.834722344065</v>
+        <v>2045.708021751251</v>
       </c>
     </row>
     <row r="5">
@@ -891,7 +979,7 @@
         <v>2033</v>
       </c>
       <c r="B5" t="n">
-        <v>3802.288486162279</v>
+        <v>3281.411881252272</v>
       </c>
     </row>
     <row r="6">
@@ -899,7 +987,7 @@
         <v>2034</v>
       </c>
       <c r="B6" t="n">
-        <v>5339.357782067029</v>
+        <v>4514.028502171678</v>
       </c>
     </row>
     <row r="7">
@@ -907,7 +995,7 @@
         <v>2035</v>
       </c>
       <c r="B7" t="n">
-        <v>6894.157904940788</v>
+        <v>5746.500988051263</v>
       </c>
     </row>
     <row r="8">
@@ -915,7 +1003,7 @@
         <v>2036</v>
       </c>
       <c r="B8" t="n">
-        <v>8886.209318660736</v>
+        <v>7001.111673184272</v>
       </c>
     </row>
     <row r="9">
@@ -923,7 +1011,7 @@
         <v>2037</v>
       </c>
       <c r="B9" t="n">
-        <v>10942.87052212597</v>
+        <v>8622.457111520587</v>
       </c>
     </row>
     <row r="10">
@@ -931,7 +1019,7 @@
         <v>2038</v>
       </c>
       <c r="B10" t="n">
-        <v>13762.28455426672</v>
+        <v>10870.14146510213</v>
       </c>
     </row>
     <row r="11">
@@ -939,7 +1027,7 @@
         <v>2039</v>
       </c>
       <c r="B11" t="n">
-        <v>16581.74424534588</v>
+        <v>13117.90525630524</v>
       </c>
     </row>
     <row r="12">
@@ -947,7 +1035,7 @@
         <v>2040</v>
       </c>
       <c r="B12" t="n">
-        <v>19401.34204290319</v>
+        <v>15365.79889716131</v>
       </c>
     </row>
     <row r="13">
@@ -955,7 +1043,7 @@
         <v>2041</v>
       </c>
       <c r="B13" t="n">
-        <v>22228.66476593326</v>
+        <v>17619.49245708499</v>
       </c>
     </row>
     <row r="14">
@@ -963,7 +1051,7 @@
         <v>2042</v>
       </c>
       <c r="B14" t="n">
-        <v>25048.26256349056</v>
+        <v>19867.46126914401</v>
       </c>
     </row>
     <row r="15">
@@ -971,7 +1059,7 @@
         <v>2043</v>
       </c>
       <c r="B15" t="n">
-        <v>27098.68883165535</v>
+        <v>22115.08578061984</v>
       </c>
     </row>
     <row r="16">
@@ -979,7 +1067,7 @@
         <v>2044</v>
       </c>
       <c r="B16" t="n">
-        <v>29149.59616059932</v>
+        <v>24434.35790656858</v>
       </c>
     </row>
     <row r="17">
@@ -987,7 +1075,7 @@
         <v>2045</v>
       </c>
       <c r="B17" t="n">
-        <v>31206.15780847576</v>
+        <v>26512.00400623473</v>
       </c>
     </row>
     <row r="18">
@@ -995,7 +1083,7 @@
         <v>2046</v>
       </c>
       <c r="B18" t="n">
-        <v>33257.19971903536</v>
+        <v>28129.74250700068</v>
       </c>
     </row>
     <row r="19">
@@ -1003,7 +1091,31 @@
         <v>2047</v>
       </c>
       <c r="B19" t="n">
-        <v>34923.20299695621</v>
+        <v>29747.53028628441</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B20" t="n">
+        <v>31365.20085935633</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B21" t="n">
+        <v>32987.36707041616</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B22" t="n">
+        <v>34492.79940537025</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +1129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1042,7 +1154,7 @@
         <v>2030</v>
       </c>
       <c r="B2" t="n">
-        <v>515.8347223440652</v>
+        <v>408.9581304771178</v>
       </c>
     </row>
     <row r="3">
@@ -1050,7 +1162,7 @@
         <v>2031</v>
       </c>
       <c r="B3" t="n">
-        <v>1284.348131251097</v>
+        <v>1018.223551505877</v>
       </c>
     </row>
     <row r="4">
@@ -1058,7 +1170,7 @@
         <v>2032</v>
       </c>
       <c r="B4" t="n">
-        <v>2515.834722344065</v>
+        <v>2045.708021751251</v>
       </c>
     </row>
     <row r="5">
@@ -1066,7 +1178,7 @@
         <v>2033</v>
       </c>
       <c r="B5" t="n">
-        <v>4572.882397908923</v>
+        <v>3884.708584548976</v>
       </c>
     </row>
     <row r="6">
@@ -1074,7 +1186,7 @@
         <v>2034</v>
       </c>
       <c r="B6" t="n">
-        <v>6878.487453939287</v>
+        <v>5718.98763398018</v>
       </c>
     </row>
     <row r="7">
@@ -1082,7 +1194,7 @@
         <v>2035</v>
       </c>
       <c r="B7" t="n">
-        <v>9201.843463810765</v>
+        <v>7553.149796348535</v>
       </c>
     </row>
     <row r="8">
@@ -1090,7 +1202,7 @@
         <v>2036</v>
       </c>
       <c r="B8" t="n">
-        <v>11962.45076452843</v>
+        <v>9409.450157970316</v>
       </c>
     </row>
     <row r="9">
@@ -1098,7 +1210,7 @@
         <v>2037</v>
       </c>
       <c r="B9" t="n">
-        <v>14789.7734875585</v>
+        <v>11634.13373766249</v>
       </c>
     </row>
     <row r="10">
@@ -1106,7 +1218,7 @@
         <v>2038</v>
       </c>
       <c r="B10" t="n">
-        <v>17815.03233480562</v>
+        <v>13881.85941608445</v>
       </c>
     </row>
     <row r="11">
@@ -1114,7 +1226,7 @@
         <v>2039</v>
       </c>
       <c r="B11" t="n">
-        <v>20891.3782886815</v>
+        <v>16201.89501145963</v>
       </c>
     </row>
     <row r="12">
@@ -1122,7 +1234,7 @@
         <v>2040</v>
       </c>
       <c r="B12" t="n">
-        <v>25239.30795130547</v>
+        <v>19741.46952342551</v>
       </c>
     </row>
     <row r="13">
@@ -1130,7 +1242,7 @@
         <v>2041</v>
       </c>
       <c r="B13" t="n">
-        <v>29983.21882123356</v>
+        <v>23825.57011782019</v>
       </c>
     </row>
     <row r="14">
@@ -1138,7 +1250,7 @@
         <v>2042</v>
       </c>
       <c r="B14" t="n">
-        <v>34214.76697803549</v>
+        <v>27899.01258629511</v>
       </c>
     </row>
     <row r="15">
@@ -1146,7 +1258,7 @@
         <v>2043</v>
       </c>
       <c r="B15" t="n">
-        <v>38857.48342711201</v>
+        <v>31972.00520798409</v>
       </c>
     </row>
     <row r="16">
@@ -1154,7 +1266,7 @@
         <v>2044</v>
       </c>
       <c r="B16" t="n">
-        <v>43207.10757855997</v>
+        <v>36034.99308419366</v>
       </c>
     </row>
     <row r="17">
@@ -1162,7 +1274,7 @@
         <v>2045</v>
       </c>
       <c r="B17" t="n">
-        <v>47134.85676058558</v>
+        <v>40001.94910813661</v>
       </c>
     </row>
     <row r="18">
@@ -1170,7 +1282,7 @@
         <v>2046</v>
       </c>
       <c r="B18" t="n">
-        <v>50366.40491738752</v>
+        <v>43271.18792272181</v>
       </c>
     </row>
     <row r="19">
@@ -1178,7 +1290,7 @@
         <v>2047</v>
       </c>
       <c r="B19" t="n">
-        <v>53049.40641710248</v>
+        <v>46324.68813972538</v>
       </c>
     </row>
     <row r="20">
@@ -1186,7 +1298,31 @@
         <v>2048</v>
       </c>
       <c r="B20" t="n">
-        <v>54843.69731230784</v>
+        <v>48774.77288226459</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B21" t="n">
+        <v>51241.61957253295</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B22" t="n">
+        <v>53034.44628541584</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B23" t="n">
+        <v>54373.77672209026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ORBIT towing group compatibility
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Baseline-limited-ports" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Baseline-South-CA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Baseline-Central-CA" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Expanded-all-ports" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -648,4 +651,545 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cummulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B2" t="n">
+        <v>407.2304176189487</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1407.230417618949</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2416.371618750885</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4046.408984503963</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6266.177250188815</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9220.979273168934</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B8" t="n">
+        <v>12105.86042738475</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B9" t="n">
+        <v>15304.58631049695</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B10" t="n">
+        <v>17932.10799615077</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B11" t="n">
+        <v>21257.82231210306</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B12" t="n">
+        <v>24375.96813480699</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B13" t="n">
+        <v>27564.34172178803</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B14" t="n">
+        <v>29543.23725055432</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B15" t="n">
+        <v>31079.73360091929</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B16" t="n">
+        <v>32543.23725055432</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B17" t="n">
+        <v>33898.03721359599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cummulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B2" t="n">
+        <v>407.2304176189487</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1407.230417618949</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2416.371618750885</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3445.629284073075</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5066.24564964162</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6822.730240215845</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8443.038978354918</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10239.4110814471</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B10" t="n">
+        <v>12665.8387943053</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B11" t="n">
+        <v>15919.61597541799</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B12" t="n">
+        <v>19173.43735505323</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B13" t="n">
+        <v>22426.13538510296</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B14" t="n">
+        <v>24540.70647080056</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B15" t="n">
+        <v>26139.88567736691</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B16" t="n">
+        <v>27804.48371464776</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B17" t="n">
+        <v>29960.8166642758</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B18" t="n">
+        <v>31862.12245642851</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B19" t="n">
+        <v>32661.46546217721</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B20" t="n">
+        <v>33460.76642335767</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B21" t="n">
+        <v>34262.2502053107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cummulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="B2" t="n">
+        <v>407.2304176189487</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1407.230417618949</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2416.371618750885</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4046.408984503963</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6266.177250188815</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8621.841047329388</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10841.32899203481</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B9" t="n">
+        <v>13238.52188856064</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B10" t="n">
+        <v>15664.99058214565</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B11" t="n">
+        <v>18984.76240666921</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B12" t="n">
+        <v>23522.17776208614</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B13" t="n">
+        <v>28601.34058502495</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B14" t="n">
+        <v>33669.33764385931</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B15" t="n">
+        <v>38737.44076710031</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B16" t="n">
+        <v>43795.9591328035</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B17" t="n">
+        <v>48604.10730007126</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B18" t="n">
+        <v>51764.77980879939</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B19" t="n">
+        <v>53198.10201660736</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B20" t="n">
+        <v>53997.44502235606</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B21" t="n">
+        <v>54808.9430894309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Relocate legend on plot_sumary
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -8,6 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="Baseline-Low" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Baseline-Mid (SC)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Baseline-Mid (CC)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Moderate-Low" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Moderate-Mid (SC)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Expanded-High" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +430,770 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1298.617392332037</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2276.697484881295</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3261.977426753822</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4242.837463853284</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5218.916186298174</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6190.215016890826</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7163.164940367873</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8214.825658884853</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9520.265118171012</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10822.57966268448</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12153.38094730442</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B13" t="n">
+        <v>13478.5894208557</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B14" t="n">
+        <v>14786.29677183206</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16095.7060532272</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B16" t="n">
+        <v>17437.07746674893</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B17" t="n">
+        <v>18749.47402992389</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20061.73197624848</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B19" t="n">
+        <v>21396.43398280865</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B20" t="n">
+        <v>22711.40342408068</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B21" t="n">
+        <v>23999.28333973481</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B22" t="n">
+        <v>24872.50337888572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1154.17065076776</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1823.443388267057</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2817.795556914285</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4127.643693473954</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6195.251873359175</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8343.191712963724</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10474.009708605</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B9" t="n">
+        <v>12606.2351429245</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B10" t="n">
+        <v>14747.74403663507</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B11" t="n">
+        <v>16442.10526315789</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B12" t="n">
+        <v>17880.86069368357</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B13" t="n">
+        <v>19442.90448930401</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20880.86069368357</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B15" t="n">
+        <v>22442.90448930401</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B16" t="n">
+        <v>23546.14203467721</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B17" t="n">
+        <v>24748.92988929889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1154.17065076776</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1823.443388267057</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2331.174317093777</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3155.730780061955</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4250.915979584492</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5426.359516616314</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6442.105263157895</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B9" t="n">
+        <v>7928.690832229717</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9415.276401301538</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10901.83643400882</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12390.5272398039</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B13" t="n">
+        <v>13873.61692525089</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B14" t="n">
+        <v>15356.2881468058</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16830.27245653833</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B16" t="n">
+        <v>18406.88788507601</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20204.79053293633</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B18" t="n">
+        <v>21101.2252042007</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B19" t="n">
+        <v>21740.08168028005</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B20" t="n">
+        <v>22393.24996233238</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B21" t="n">
+        <v>23051.34918903193</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B22" t="n">
+        <v>23688.48643537712</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2052</v>
+      </c>
+      <c r="B23" t="n">
+        <v>24338.09092282133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1298.617392332037</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2609.78534530162</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4092.65776437349</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5572.232441022234</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B6" t="n">
+        <v>7048.311163467123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8519.609994059774</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9993.929780550521</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B9" t="n">
+        <v>11665.62301399959</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B10" t="n">
+        <v>14312.00153677913</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B11" t="n">
+        <v>16942.74542067324</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B12" t="n">
+        <v>19634.15229886452</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B13" t="n">
+        <v>22285.46292307787</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B14" t="n">
+        <v>24567.28604477605</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B15" t="n">
+        <v>26095.7060532272</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B16" t="n">
+        <v>27437.07746674893</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B17" t="n">
+        <v>28749.47402992389</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2047</v>
+      </c>
+      <c r="B18" t="n">
+        <v>30061.73197624848</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B19" t="n">
+        <v>31396.43398280865</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B20" t="n">
+        <v>32711.40342408068</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B21" t="n">
+        <v>33999.28333973481</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B22" t="n">
+        <v>34872.50337888572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -447,146 +1216,345 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>402.1612748785993</v>
+        <v>1154.17065076776</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1607.989803607023</v>
+        <v>2156.531248687382</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>2813.874003262026</v>
+        <v>3648.475894533953</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>4023.089311171367</v>
+        <v>5457.038670642904</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>5229.000752119207</v>
+        <v>7538.709090501497</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>6434.912193067049</v>
+        <v>9700.711170079419</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>7640.82363401489</v>
+        <v>11702.26015237906</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>9139.900050128464</v>
+        <v>13804.96388886606</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>10750.18477457502</v>
+        <v>16619.91626680589</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>12363.52933297643</v>
+        <v>19420.43010715657</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>13975.05312759863</v>
+        <v>22377.76500531643</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>15591.2960907102</v>
+        <v>25349.25290401158</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>17204.36067997044</v>
+        <v>27962.22515081275</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>18814.92327365308</v>
+        <v>29832.53836002874</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>20429.27099695094</v>
+        <v>31595.74564221231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>22042.60355468518</v>
+        <v>33435.67074317917</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>23658.50503557239</v>
+        <v>34336.27850777828</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B19" t="n">
+        <v>34997.80999848965</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Capacity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2031</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1154.17065076776</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2156.531248687382</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2033</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3648.475894533953</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2034</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5457.038670642904</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2035</v>
+      </c>
+      <c r="B6" t="n">
+        <v>7538.709090501497</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9700.711170079419</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2037</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11702.26015237906</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2038</v>
+      </c>
+      <c r="B9" t="n">
+        <v>13804.96388886606</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2039</v>
+      </c>
+      <c r="B10" t="n">
+        <v>16619.91626680589</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2040</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20304.64063347235</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B12" t="n">
+        <v>24579.09341860057</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2042</v>
+      </c>
+      <c r="B13" t="n">
+        <v>28843.57024718502</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2043</v>
+      </c>
+      <c r="B14" t="n">
+        <v>33106.59742401617</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2044</v>
+      </c>
+      <c r="B15" t="n">
+        <v>37420.80771006332</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B16" t="n">
+        <v>41796.22882817144</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2046</v>
+      </c>
+      <c r="B17" t="n">
+        <v>46262.73980836057</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>2047</v>
       </c>
+      <c r="B18" t="n">
+        <v>49818.24025444769</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2048</v>
+      </c>
       <c r="B19" t="n">
-        <v>24882.93449136099</v>
+        <v>52309.18932698269</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B20" t="n">
+        <v>53330.86419753086</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2050</v>
+      </c>
+      <c r="B21" t="n">
+        <v>53986.30751964085</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2051</v>
+      </c>
+      <c r="B22" t="n">
+        <v>54630.01322168356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed O&M window typo
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         <v>2032</v>
       </c>
       <c r="B2" t="n">
-        <v>1597.812496376989</v>
+        <v>1627.807136655092</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         <v>2033</v>
       </c>
       <c r="B3" t="n">
-        <v>2292.438725300954</v>
+        <v>2334.585451983126</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +471,7 @@
         <v>2034</v>
       </c>
       <c r="B4" t="n">
-        <v>3014.698115520799</v>
+        <v>3077.290613913541</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
         <v>2035</v>
       </c>
       <c r="B5" t="n">
-        <v>3736.957505740643</v>
+        <v>3812.44496461266</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         <v>2036</v>
       </c>
       <c r="B6" t="n">
-        <v>4402.676088508074</v>
+        <v>4488.452146064634</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         <v>2037</v>
       </c>
       <c r="B7" t="n">
-        <v>5130.675126629729</v>
+        <v>5253.728661349983</v>
       </c>
     </row>
     <row r="8">
@@ -503,7 +503,7 @@
         <v>2038</v>
       </c>
       <c r="B8" t="n">
-        <v>5856.685096341215</v>
+        <v>6015.259188441078</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>2039</v>
       </c>
       <c r="B9" t="n">
-        <v>6583.101468935075</v>
+        <v>6751.250087432547</v>
       </c>
     </row>
     <row r="10">
@@ -519,7 +519,7 @@
         <v>2040</v>
       </c>
       <c r="B10" t="n">
-        <v>7311.280984164358</v>
+        <v>7487.240986424014</v>
       </c>
     </row>
     <row r="11">
@@ -527,7 +527,7 @@
         <v>2041</v>
       </c>
       <c r="B11" t="n">
-        <v>8099.947238564641</v>
+        <v>8341.181536593529</v>
       </c>
     </row>
     <row r="12">
@@ -535,7 +535,7 @@
         <v>2042</v>
       </c>
       <c r="B12" t="n">
-        <v>9071.566404721138</v>
+        <v>9390.738377412039</v>
       </c>
     </row>
     <row r="13">
@@ -543,7 +543,7 @@
         <v>2043</v>
       </c>
       <c r="B13" t="n">
-        <v>10045.2792825567</v>
+        <v>10368.61519730597</v>
       </c>
     </row>
     <row r="14">
@@ -551,7 +551,7 @@
         <v>2044</v>
       </c>
       <c r="B14" t="n">
-        <v>11032.6732441267</v>
+        <v>11432.22740586152</v>
       </c>
     </row>
     <row r="15">
@@ -559,7 +559,7 @@
         <v>2045</v>
       </c>
       <c r="B15" t="n">
-        <v>11965.46927124592</v>
+        <v>12443.95682558234</v>
       </c>
     </row>
     <row r="16">
@@ -567,7 +567,7 @@
         <v>2046</v>
       </c>
       <c r="B16" t="n">
-        <v>12876.99936199469</v>
+        <v>13407.65323706305</v>
       </c>
     </row>
     <row r="17">
@@ -575,7 +575,7 @@
         <v>2047</v>
       </c>
       <c r="B17" t="n">
-        <v>13860.47551656237</v>
+        <v>14461.78947628179</v>
       </c>
     </row>
     <row r="18">
@@ -583,7 +583,7 @@
         <v>2048</v>
       </c>
       <c r="B18" t="n">
-        <v>14942.16082523586</v>
+        <v>15465.28774702235</v>
       </c>
     </row>
     <row r="19">
@@ -591,7 +591,7 @@
         <v>2049</v>
       </c>
       <c r="B19" t="n">
-        <v>15933.77070559165</v>
+        <v>16436.10267932832</v>
       </c>
     </row>
     <row r="20">
@@ -599,7 +599,7 @@
         <v>2050</v>
       </c>
       <c r="B20" t="n">
-        <v>16912.31228931549</v>
+        <v>17488.43301133983</v>
       </c>
     </row>
     <row r="21">
@@ -607,7 +607,7 @@
         <v>2051</v>
       </c>
       <c r="B21" t="n">
-        <v>17841.72759829751</v>
+        <v>18480.05251112411</v>
       </c>
     </row>
     <row r="22">
@@ -615,7 +615,7 @@
         <v>2052</v>
       </c>
       <c r="B22" t="n">
-        <v>18757.53496192253</v>
+        <v>19441.14378569984</v>
       </c>
     </row>
     <row r="23">
@@ -623,7 +623,7 @@
         <v>2053</v>
       </c>
       <c r="B23" t="n">
-        <v>19730.33601452901</v>
+        <v>20491.14363214689</v>
       </c>
     </row>
     <row r="24">
@@ -631,7 +631,7 @@
         <v>2054</v>
       </c>
       <c r="B24" t="n">
-        <v>20835.06377058314</v>
+        <v>21482.74501084779</v>
       </c>
     </row>
     <row r="25">
@@ -639,7 +639,7 @@
         <v>2055</v>
       </c>
       <c r="B25" t="n">
-        <v>21850.45780503368</v>
+        <v>22443.77372745027</v>
       </c>
     </row>
     <row r="26">
@@ -647,7 +647,7 @@
         <v>2056</v>
       </c>
       <c r="B26" t="n">
-        <v>22855.6491428782</v>
+        <v>23500.84207744599</v>
       </c>
     </row>
     <row r="27">
@@ -655,15 +655,7 @@
         <v>2057</v>
       </c>
       <c r="B27" t="n">
-        <v>23918.39658783402</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>2058</v>
-      </c>
-      <c r="B28" t="n">
-        <v>24988.05747340922</v>
+        <v>24592.92580724673</v>
       </c>
     </row>
   </sheetData>
@@ -702,7 +694,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>965.8743233702048</v>
+        <v>1014.686248331108</v>
       </c>
     </row>
     <row r="3">
@@ -710,7 +702,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1689.103318427865</v>
+        <v>1723.928200563715</v>
       </c>
     </row>
     <row r="4">
@@ -718,7 +710,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>2627.700713157349</v>
+        <v>2652.480900977594</v>
       </c>
     </row>
     <row r="5">
@@ -726,7 +718,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>3667.242100062979</v>
+        <v>3737.659267944707</v>
       </c>
     </row>
     <row r="6">
@@ -734,7 +726,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>5222.394460507738</v>
+        <v>5405.037494671253</v>
       </c>
     </row>
     <row r="7">
@@ -742,7 +734,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>6897.649509334109</v>
+        <v>7286.013900313775</v>
       </c>
     </row>
     <row r="8">
@@ -750,7 +742,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>8698.221264752301</v>
+        <v>9144.594764214053</v>
       </c>
     </row>
     <row r="9">
@@ -758,7 +750,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>10601.89787275117</v>
+        <v>10954.11508666184</v>
       </c>
     </row>
     <row r="10">
@@ -766,7 +758,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>12547.53657766244</v>
+        <v>12768.9411359356</v>
       </c>
     </row>
     <row r="11">
@@ -774,7 +766,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>14470.58531612279</v>
+        <v>14623.6582912613</v>
       </c>
     </row>
     <row r="12">
@@ -782,7 +774,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>16389.33804043258</v>
+        <v>16559.53882147466</v>
       </c>
     </row>
     <row r="13">
@@ -790,7 +782,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>18304.24857340841</v>
+        <v>18470.18061703362</v>
       </c>
     </row>
     <row r="14">
@@ -798,7 +790,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>20159.49635626794</v>
+        <v>20290.75680477099</v>
       </c>
     </row>
     <row r="15">
@@ -806,7 +798,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>22143.17616876253</v>
+        <v>22268.49720168707</v>
       </c>
     </row>
     <row r="16">
@@ -814,7 +806,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>23319.0264776424</v>
+        <v>23376.74780385629</v>
       </c>
     </row>
     <row r="17">
@@ -822,7 +814,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>24414.43135452917</v>
+        <v>24496.32143330742</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +853,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>965.8743233702048</v>
+        <v>1014.686248331108</v>
       </c>
     </row>
     <row r="3">
@@ -869,7 +861,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1689.103318427865</v>
+        <v>1723.928200563715</v>
       </c>
     </row>
     <row r="4">
@@ -877,7 +869,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>2277.084020545686</v>
+        <v>2291.103519976236</v>
       </c>
     </row>
     <row r="5">
@@ -885,7 +877,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>2966.966683945148</v>
+        <v>3015.891875835438</v>
       </c>
     </row>
     <row r="6">
@@ -893,7 +885,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>3822.522059552372</v>
+        <v>3965.591786236091</v>
       </c>
     </row>
     <row r="7">
@@ -901,7 +893,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>4798.514730947163</v>
+        <v>5140.600315955766</v>
       </c>
     </row>
     <row r="8">
@@ -909,7 +901,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>5898.013936495851</v>
+        <v>6294.860774066269</v>
       </c>
     </row>
     <row r="9">
@@ -917,7 +909,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>7455.448848532084</v>
+        <v>7757.582049913518</v>
       </c>
     </row>
     <row r="10">
@@ -925,7 +917,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>8982.369222513043</v>
+        <v>9142.772446536506</v>
       </c>
     </row>
     <row r="11">
@@ -933,7 +925,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>10463.42830343166</v>
+        <v>10542.66790702044</v>
       </c>
     </row>
     <row r="12">
@@ -941,7 +933,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>11863.73326517501</v>
+        <v>11967.6337443147</v>
       </c>
     </row>
     <row r="13">
@@ -949,7 +941,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>13260.73911560553</v>
+        <v>13388.17813356356</v>
       </c>
     </row>
     <row r="14">
@@ -957,7 +949,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>14650.5183855751</v>
+        <v>14782.15159882103</v>
       </c>
     </row>
     <row r="15">
@@ -965,7 +957,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>16039.09184192712</v>
+        <v>16176.12506407851</v>
       </c>
     </row>
     <row r="16">
@@ -973,7 +965,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>17427.86384758585</v>
+        <v>17583.27467643587</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +973,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>18901.45807818327</v>
+        <v>19116.5632392959</v>
       </c>
     </row>
     <row r="18">
@@ -989,7 +981,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>19865.21607736476</v>
+        <v>20041.31234199035</v>
       </c>
     </row>
     <row r="19">
@@ -997,7 +989,7 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>20359.5892595191</v>
+        <v>20544.64490921627</v>
       </c>
     </row>
     <row r="20">
@@ -1005,7 +997,7 @@
         <v>2049</v>
       </c>
       <c r="B20" t="n">
-        <v>20919.82907073155</v>
+        <v>21049.66753396935</v>
       </c>
     </row>
     <row r="21">
@@ -1013,7 +1005,7 @@
         <v>2050</v>
       </c>
       <c r="B21" t="n">
-        <v>21446.58056068091</v>
+        <v>21556.17230413414</v>
       </c>
     </row>
     <row r="22">
@@ -1021,7 +1013,7 @@
         <v>2051</v>
       </c>
       <c r="B22" t="n">
-        <v>21967.97809654187</v>
+        <v>22064.10408042578</v>
       </c>
     </row>
     <row r="23">
@@ -1029,7 +1021,7 @@
         <v>2052</v>
       </c>
       <c r="B23" t="n">
-        <v>22481.43810750673</v>
+        <v>22582.14074512123</v>
       </c>
     </row>
     <row r="24">
@@ -1037,7 +1029,7 @@
         <v>2053</v>
       </c>
       <c r="B24" t="n">
-        <v>22995.78404965453</v>
+        <v>23102.96673658975</v>
       </c>
     </row>
     <row r="25">
@@ -1045,7 +1037,7 @@
         <v>2054</v>
       </c>
       <c r="B25" t="n">
-        <v>23509.02273259902</v>
+        <v>23627.98921186694</v>
       </c>
     </row>
     <row r="26">
@@ -1053,7 +1045,7 @@
         <v>2055</v>
       </c>
       <c r="B26" t="n">
-        <v>24021.90201729107</v>
+        <v>24149.63952874978</v>
       </c>
     </row>
     <row r="27">
@@ -1061,7 +1053,7 @@
         <v>2056</v>
       </c>
       <c r="B27" t="n">
-        <v>24526.80115273775</v>
+        <v>24663.09126077018</v>
       </c>
     </row>
   </sheetData>
@@ -1075,7 +1067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1100,7 +1092,7 @@
         <v>2032</v>
       </c>
       <c r="B2" t="n">
-        <v>1880.396118060956</v>
+        <v>1919.734452711094</v>
       </c>
     </row>
     <row r="3">
@@ -1108,7 +1100,7 @@
         <v>2033</v>
       </c>
       <c r="B3" t="n">
-        <v>2997.167675704645</v>
+        <v>3062.61643202483</v>
       </c>
     </row>
     <row r="4">
@@ -1116,7 +1108,7 @@
         <v>2034</v>
       </c>
       <c r="B4" t="n">
-        <v>4140.606571987084</v>
+        <v>4245.667383870446</v>
       </c>
     </row>
     <row r="5">
@@ -1124,7 +1116,7 @@
         <v>2035</v>
       </c>
       <c r="B5" t="n">
-        <v>5284.486022850909</v>
+        <v>5430.236879244304</v>
       </c>
     </row>
     <row r="6">
@@ -1132,7 +1124,7 @@
         <v>2036</v>
       </c>
       <c r="B6" t="n">
-        <v>6371.824666262321</v>
+        <v>6552.617506566201</v>
       </c>
     </row>
     <row r="7">
@@ -1140,7 +1132,7 @@
         <v>2037</v>
       </c>
       <c r="B7" t="n">
-        <v>7512.384215834248</v>
+        <v>7748.14480555061</v>
       </c>
     </row>
     <row r="8">
@@ -1148,7 +1140,7 @@
         <v>2038</v>
       </c>
       <c r="B8" t="n">
-        <v>8649.025601661611</v>
+        <v>8938.750567751422</v>
       </c>
     </row>
     <row r="9">
@@ -1156,7 +1148,7 @@
         <v>2039</v>
       </c>
       <c r="B9" t="n">
-        <v>10412.55107551933</v>
+        <v>10737.50609513517</v>
       </c>
     </row>
     <row r="10">
@@ -1164,7 +1156,7 @@
         <v>2040</v>
       </c>
       <c r="B10" t="n">
-        <v>12276.91404730843</v>
+        <v>12560.10695459791</v>
       </c>
     </row>
     <row r="11">
@@ -1172,7 +1164,7 @@
         <v>2041</v>
       </c>
       <c r="B11" t="n">
-        <v>14141.10452553871</v>
+        <v>14502.05260734156</v>
       </c>
     </row>
     <row r="12">
@@ -1180,7 +1172,7 @@
         <v>2042</v>
       </c>
       <c r="B12" t="n">
-        <v>16179.71701745467</v>
+        <v>16677.1357781006</v>
       </c>
     </row>
     <row r="13">
@@ -1188,7 +1180,7 @@
         <v>2043</v>
       </c>
       <c r="B13" t="n">
-        <v>18228.66543000197</v>
+        <v>18863.16687652341</v>
       </c>
     </row>
     <row r="14">
@@ -1196,7 +1188,7 @@
         <v>2044</v>
       </c>
       <c r="B14" t="n">
-        <v>20294.19592310377</v>
+        <v>20901.46783272906</v>
       </c>
     </row>
     <row r="15">
@@ -1204,7 +1196,7 @@
         <v>2045</v>
       </c>
       <c r="B15" t="n">
-        <v>21870.64989702448</v>
+        <v>22443.95682558234</v>
       </c>
     </row>
     <row r="16">
@@ -1212,7 +1204,7 @@
         <v>2046</v>
       </c>
       <c r="B16" t="n">
-        <v>22876.99936199469</v>
+        <v>23407.65323706305</v>
       </c>
     </row>
     <row r="17">
@@ -1220,7 +1212,7 @@
         <v>2047</v>
       </c>
       <c r="B17" t="n">
-        <v>23860.47551656237</v>
+        <v>24461.78947628179</v>
       </c>
     </row>
     <row r="18">
@@ -1228,7 +1220,7 @@
         <v>2048</v>
       </c>
       <c r="B18" t="n">
-        <v>24942.16082523586</v>
+        <v>25465.28774702235</v>
       </c>
     </row>
     <row r="19">
@@ -1236,7 +1228,7 @@
         <v>2049</v>
       </c>
       <c r="B19" t="n">
-        <v>25933.77070559165</v>
+        <v>26436.10267932832</v>
       </c>
     </row>
     <row r="20">
@@ -1244,7 +1236,7 @@
         <v>2050</v>
       </c>
       <c r="B20" t="n">
-        <v>26912.31228931549</v>
+        <v>27488.43301133983</v>
       </c>
     </row>
     <row r="21">
@@ -1252,7 +1244,7 @@
         <v>2051</v>
       </c>
       <c r="B21" t="n">
-        <v>27841.72759829751</v>
+        <v>28480.05251112411</v>
       </c>
     </row>
     <row r="22">
@@ -1260,7 +1252,7 @@
         <v>2052</v>
       </c>
       <c r="B22" t="n">
-        <v>28757.53496192253</v>
+        <v>29441.14378569984</v>
       </c>
     </row>
     <row r="23">
@@ -1268,7 +1260,7 @@
         <v>2053</v>
       </c>
       <c r="B23" t="n">
-        <v>29730.33601452901</v>
+        <v>30491.14363214689</v>
       </c>
     </row>
     <row r="24">
@@ -1276,7 +1268,7 @@
         <v>2054</v>
       </c>
       <c r="B24" t="n">
-        <v>30835.06377058314</v>
+        <v>31482.74501084779</v>
       </c>
     </row>
     <row r="25">
@@ -1284,7 +1276,7 @@
         <v>2055</v>
       </c>
       <c r="B25" t="n">
-        <v>31850.45780503368</v>
+        <v>32443.77372745027</v>
       </c>
     </row>
     <row r="26">
@@ -1292,7 +1284,7 @@
         <v>2056</v>
       </c>
       <c r="B26" t="n">
-        <v>32855.6491428782</v>
+        <v>33500.842077446</v>
       </c>
     </row>
     <row r="27">
@@ -1300,15 +1292,7 @@
         <v>2057</v>
       </c>
       <c r="B27" t="n">
-        <v>33918.39658783402</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>2058</v>
-      </c>
-      <c r="B28" t="n">
-        <v>34988.05747340922</v>
+        <v>34592.92580724673</v>
       </c>
     </row>
   </sheetData>
@@ -1347,7 +1331,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>965.8743233702048</v>
+        <v>1014.686248331108</v>
       </c>
     </row>
     <row r="3">
@@ -1355,7 +1339,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1971.686940111833</v>
+        <v>2015.855516619717</v>
       </c>
     </row>
     <row r="4">
@@ -1363,7 +1347,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>3332.443659117986</v>
+        <v>3380.511881019298</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1355,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>4793.17850940393</v>
+        <v>4906.036037901612</v>
       </c>
     </row>
     <row r="6">
@@ -1379,7 +1363,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>6419.964861237849</v>
+        <v>6662.083208256897</v>
       </c>
     </row>
     <row r="7">
@@ -1387,7 +1371,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>8166.818114745345</v>
+        <v>8628.686858723344</v>
       </c>
     </row>
     <row r="8">
@@ -1395,7 +1379,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>10029.07517655952</v>
+        <v>10559.36558821764</v>
       </c>
     </row>
     <row r="9">
@@ -1403,7 +1387,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>11962.7219678613</v>
+        <v>12408.56885251923</v>
       </c>
     </row>
     <row r="10">
@@ -1411,7 +1395,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>14485.11147803104</v>
+        <v>14808.69772646339</v>
       </c>
     </row>
     <row r="11">
@@ -1419,7 +1403,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>17054.62431890857</v>
+        <v>17232.67193248653</v>
       </c>
     </row>
     <row r="12">
@@ -1427,7 +1411,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>19470.74120351153</v>
+        <v>19660.32550125241</v>
       </c>
     </row>
     <row r="13">
@@ -1435,7 +1419,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>21871.9671823035</v>
+        <v>22120.83530867213</v>
       </c>
     </row>
     <row r="14">
@@ -1443,7 +1427,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>24281.5283410134</v>
+        <v>24664.06972337513</v>
       </c>
     </row>
     <row r="15">
@@ -1451,7 +1435,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>26735.00159615793</v>
+        <v>27025.60835442773</v>
       </c>
     </row>
     <row r="16">
@@ -1459,7 +1443,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>28834.99359703491</v>
+        <v>29028.31723864588</v>
       </c>
     </row>
     <row r="17">
@@ -1467,7 +1451,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>30479.61426846446</v>
+        <v>30613.57506482587</v>
       </c>
     </row>
     <row r="18">
@@ -1475,7 +1459,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>31528.28293508141</v>
+        <v>31574.98171177761</v>
       </c>
     </row>
     <row r="19">
@@ -1483,7 +1467,7 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>31991.38295622753</v>
+        <v>32033.85980095197</v>
       </c>
     </row>
     <row r="20">
@@ -1491,7 +1475,7 @@
         <v>2049</v>
       </c>
       <c r="B20" t="n">
-        <v>32468.27810972298</v>
+        <v>32508.97879705755</v>
       </c>
     </row>
     <row r="21">
@@ -1499,7 +1483,7 @@
         <v>2050</v>
       </c>
       <c r="B21" t="n">
-        <v>32944.10646387833</v>
+        <v>32982.79965382951</v>
       </c>
     </row>
     <row r="22">
@@ -1507,7 +1491,7 @@
         <v>2051</v>
       </c>
       <c r="B22" t="n">
-        <v>33433.27915709242</v>
+        <v>33465.58570483124</v>
       </c>
     </row>
     <row r="23">
@@ -1515,7 +1499,7 @@
         <v>2052</v>
       </c>
       <c r="B23" t="n">
-        <v>33924.22798856694</v>
+        <v>33948.70946393117</v>
       </c>
     </row>
     <row r="24">
@@ -1523,7 +1507,7 @@
         <v>2053</v>
       </c>
       <c r="B24" t="n">
-        <v>34420.93339374717</v>
+        <v>34445.76877234803</v>
       </c>
     </row>
     <row r="25">
@@ -1531,7 +1515,7 @@
         <v>2054</v>
       </c>
       <c r="B25" t="n">
-        <v>34917.08201178069</v>
+        <v>34942.95930529542</v>
       </c>
     </row>
   </sheetData>
@@ -1570,7 +1554,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>965.8743233702048</v>
+        <v>1014.686248331108</v>
       </c>
     </row>
     <row r="3">
@@ -1578,7 +1562,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1689.103318427865</v>
+        <v>1723.928200563715</v>
       </c>
     </row>
     <row r="4">
@@ -1586,7 +1570,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>3379.14846313587</v>
+        <v>3437.346855886964</v>
       </c>
     </row>
     <row r="5">
@@ -1594,7 +1578,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>5168.084464091117</v>
+        <v>5305.246735263695</v>
       </c>
     </row>
     <row r="6">
@@ -1602,7 +1586,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>7144.224522619969</v>
+        <v>7409.072479854041</v>
       </c>
     </row>
     <row r="7">
@@ -1610,7 +1594,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>9661.783176324769</v>
+        <v>10147.91602383643</v>
       </c>
     </row>
     <row r="8">
@@ -1618,7 +1602,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>12348.12427674307</v>
+        <v>12964.92538126792</v>
       </c>
     </row>
     <row r="9">
@@ -1626,7 +1610,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>15392.6850176917</v>
+        <v>16027.06846302629</v>
       </c>
     </row>
     <row r="10">
@@ -1634,7 +1618,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>18982.75449040498</v>
+        <v>19469.91728751813</v>
       </c>
     </row>
     <row r="11">
@@ -1642,7 +1626,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>22962.67459402401</v>
+        <v>23302.33724353648</v>
       </c>
     </row>
     <row r="12">
@@ -1650,7 +1634,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>27095.67224265078</v>
+        <v>27506.59834337482</v>
       </c>
     </row>
     <row r="13">
@@ -1658,7 +1642,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>31484.56650556875</v>
+        <v>32004.84905238706</v>
       </c>
     </row>
     <row r="14">
@@ -1666,7 +1650,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>35838.13129253995</v>
+        <v>36447.59295925179</v>
       </c>
     </row>
     <row r="15">
@@ -1674,7 +1658,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>40247.37714155496</v>
+        <v>40904.52398475842</v>
       </c>
     </row>
     <row r="16">
@@ -1682,7 +1666,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>44574.63642465616</v>
+        <v>45300.97908368556</v>
       </c>
     </row>
     <row r="17">
@@ -1690,7 +1674,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>48881.83251701761</v>
+        <v>49297.02427482433</v>
       </c>
     </row>
     <row r="18">
@@ -1698,7 +1682,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>52271.91497318125</v>
+        <v>52622.46709841703</v>
       </c>
     </row>
     <row r="19">
@@ -1706,7 +1690,7 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>54471.82418046514</v>
+        <v>54572.09618688664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deployment and gantt chart formatting
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Baseline-Low" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Baseline-Mid (SC)" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,210 +447,130 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>1627.807136655092</v>
+        <v>1014.686248331108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>2334.585451983126</v>
+        <v>1723.928200563715</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>3077.290613913541</v>
+        <v>2652.480900977594</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>3812.44496461266</v>
+        <v>3737.659267944707</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>4488.452146064634</v>
+        <v>5405.037494671253</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>5253.728661349983</v>
+        <v>7286.013900313775</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>6015.259188441078</v>
+        <v>9144.594764214053</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>6751.250087432547</v>
+        <v>10954.11508666184</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>7487.240986424014</v>
+        <v>12768.9411359356</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>8341.181536593529</v>
+        <v>14623.6582912613</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>9390.738377412039</v>
+        <v>16559.53882147466</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>10368.61519730597</v>
+        <v>18470.18061703362</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>11432.22740586152</v>
+        <v>20290.75680477099</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>12443.95682558234</v>
+        <v>22268.49720168707</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>13407.65323706305</v>
+        <v>23376.74780385629</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>14461.78947628179</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2048</v>
-      </c>
-      <c r="B18" t="n">
-        <v>15465.28774702235</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2049</v>
-      </c>
-      <c r="B19" t="n">
-        <v>16436.10267932832</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2050</v>
-      </c>
-      <c r="B20" t="n">
-        <v>17488.43301133983</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2051</v>
-      </c>
-      <c r="B21" t="n">
-        <v>18480.05251112411</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>2052</v>
-      </c>
-      <c r="B22" t="n">
-        <v>19441.14378569984</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>2053</v>
-      </c>
-      <c r="B23" t="n">
-        <v>20491.14363214689</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>2054</v>
-      </c>
-      <c r="B24" t="n">
-        <v>21482.74501084779</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>2055</v>
-      </c>
-      <c r="B25" t="n">
-        <v>22443.77372745027</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2056</v>
-      </c>
-      <c r="B26" t="n">
-        <v>23500.84207744599</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>2057</v>
-      </c>
-      <c r="B27" t="n">
-        <v>24592.92580724673</v>
+        <v>24496.32143330742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to align with ORBIT configs
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -455,7 +455,7 @@
         <v>2032</v>
       </c>
       <c r="B2" t="n">
-        <v>1789.841500945225</v>
+        <v>1677.930163750701</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         <v>2033</v>
       </c>
       <c r="B3" t="n">
-        <v>2585.23032705802</v>
+        <v>2326.82557742865</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +471,7 @@
         <v>2034</v>
       </c>
       <c r="B4" t="n">
-        <v>3385.778190742603</v>
+        <v>3071.442162774158</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
         <v>2035</v>
       </c>
       <c r="B5" t="n">
-        <v>4122.220710171389</v>
+        <v>3813.186489436427</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         <v>2036</v>
       </c>
       <c r="B6" t="n">
-        <v>4882.244586452645</v>
+        <v>4471.069388088458</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         <v>2037</v>
       </c>
       <c r="B7" t="n">
-        <v>5660.236667235732</v>
+        <v>5240.165460762002</v>
       </c>
     </row>
     <row r="8">
@@ -503,7 +503,7 @@
         <v>2038</v>
       </c>
       <c r="B8" t="n">
-        <v>6430.737169400287</v>
+        <v>5991.025415111622</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>2039</v>
       </c>
       <c r="B9" t="n">
-        <v>7197.056682430292</v>
+        <v>6738.872307978584</v>
       </c>
     </row>
     <row r="10">
@@ -519,7 +519,7 @@
         <v>2040</v>
       </c>
       <c r="B10" t="n">
-        <v>8011.364786409796</v>
+        <v>7506.872105826967</v>
       </c>
     </row>
     <row r="11">
@@ -527,7 +527,7 @@
         <v>2041</v>
       </c>
       <c r="B11" t="n">
-        <v>9010.674642253591</v>
+        <v>8364.110800979011</v>
       </c>
     </row>
     <row r="12">
@@ -535,7 +535,7 @@
         <v>2042</v>
       </c>
       <c r="B12" t="n">
-        <v>10014.49205757578</v>
+        <v>9306.301179207319</v>
       </c>
     </row>
     <row r="13">
@@ -543,7 +543,7 @@
         <v>2043</v>
       </c>
       <c r="B13" t="n">
-        <v>11016.68207515606</v>
+        <v>10277.69373079723</v>
       </c>
     </row>
     <row r="14">
@@ -551,7 +551,7 @@
         <v>2044</v>
       </c>
       <c r="B14" t="n">
-        <v>11945.78359650867</v>
+        <v>11267.92801500317</v>
       </c>
     </row>
     <row r="15">
@@ -559,7 +559,7 @@
         <v>2045</v>
       </c>
       <c r="B15" t="n">
-        <v>12869.62190811221</v>
+        <v>12340.31378137568</v>
       </c>
     </row>
     <row r="16">
@@ -567,7 +567,7 @@
         <v>2046</v>
       </c>
       <c r="B16" t="n">
-        <v>13910.76788544547</v>
+        <v>13376.62374306103</v>
       </c>
     </row>
     <row r="17">
@@ -575,7 +575,7 @@
         <v>2047</v>
       </c>
       <c r="B17" t="n">
-        <v>15071.6429396868</v>
+        <v>14556.33076731603</v>
       </c>
     </row>
     <row r="18">
@@ -583,7 +583,7 @@
         <v>2048</v>
       </c>
       <c r="B18" t="n">
-        <v>16065.49263538764</v>
+        <v>15551.27324557401</v>
       </c>
     </row>
     <row r="19">
@@ -591,7 +591,7 @@
         <v>2049</v>
       </c>
       <c r="B19" t="n">
-        <v>17049.25545867653</v>
+        <v>16541.54169241404</v>
       </c>
     </row>
     <row r="20">
@@ -599,7 +599,7 @@
         <v>2050</v>
       </c>
       <c r="B20" t="n">
-        <v>18038.76765767459</v>
+        <v>17531.30099946307</v>
       </c>
     </row>
     <row r="21">
@@ -607,7 +607,7 @@
         <v>2051</v>
       </c>
       <c r="B21" t="n">
-        <v>19030.47256176306</v>
+        <v>18553.29271574779</v>
       </c>
     </row>
     <row r="22">
@@ -615,7 +615,7 @@
         <v>2052</v>
       </c>
       <c r="B22" t="n">
-        <v>20105.18084692169</v>
+        <v>19609.45417951032</v>
       </c>
     </row>
     <row r="23">
@@ -623,7 +623,7 @@
         <v>2053</v>
       </c>
       <c r="B23" t="n">
-        <v>21159.64732010838</v>
+        <v>20778.7998683004</v>
       </c>
     </row>
     <row r="24">
@@ -631,7 +631,7 @@
         <v>2054</v>
       </c>
       <c r="B24" t="n">
-        <v>22116.49740373248</v>
+        <v>21841.76789504404</v>
       </c>
     </row>
     <row r="25">
@@ -639,7 +639,7 @@
         <v>2055</v>
       </c>
       <c r="B25" t="n">
-        <v>23075.58070431934</v>
+        <v>22937.34591886247</v>
       </c>
     </row>
     <row r="26">
@@ -647,7 +647,7 @@
         <v>2056</v>
       </c>
       <c r="B26" t="n">
-        <v>24142.16066517226</v>
+        <v>24177.53899456122</v>
       </c>
     </row>
   </sheetData>
@@ -686,7 +686,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>1020.793950850662</v>
+        <v>1106.975238711766</v>
       </c>
     </row>
     <row r="3">
@@ -694,7 +694,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1728.285742712168</v>
+        <v>1789.77180773588</v>
       </c>
     </row>
     <row r="4">
@@ -702,7 +702,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>2657.520757058101</v>
+        <v>2679.304511637657</v>
       </c>
     </row>
     <row r="5">
@@ -710,7 +710,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>3750.343603486754</v>
+        <v>3830.801807547724</v>
       </c>
     </row>
     <row r="6">
@@ -718,7 +718,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>5427.658713295086</v>
+        <v>5575.28616049561</v>
       </c>
     </row>
     <row r="7">
@@ -726,7 +726,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>7309.043095529309</v>
+        <v>7454.838220871127</v>
       </c>
     </row>
     <row r="8">
@@ -734,7 +734,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>9198.492409208895</v>
+        <v>9227.117625974732</v>
       </c>
     </row>
     <row r="9">
@@ -742,7 +742,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>11102.82935368304</v>
+        <v>11012.67880652528</v>
       </c>
     </row>
     <row r="10">
@@ -750,7 +750,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>12962.37417889951</v>
+        <v>12835.17561469777</v>
       </c>
     </row>
     <row r="11">
@@ -758,7 +758,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>14874.12441014114</v>
+        <v>14707.36400630029</v>
       </c>
     </row>
     <row r="12">
@@ -766,7 +766,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>16834.06111285813</v>
+        <v>16656.12081439872</v>
       </c>
     </row>
     <row r="13">
@@ -774,7 +774,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>18613.94028419859</v>
+        <v>18514.28368380099</v>
       </c>
     </row>
     <row r="14">
@@ -782,7 +782,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>20451.55026848424</v>
+        <v>20364.68695661856</v>
       </c>
     </row>
     <row r="15">
@@ -790,7 +790,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>22311.37586101646</v>
+        <v>22309.35690273768</v>
       </c>
     </row>
     <row r="16">
@@ -798,7 +798,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>23382.21288438006</v>
+        <v>23382.02691704847</v>
       </c>
     </row>
     <row r="17">
@@ -806,7 +806,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>24502.3583666581</v>
+        <v>24582.78133046177</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,7 +845,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>1020.793950850662</v>
+        <v>1106.975238711766</v>
       </c>
     </row>
     <row r="3">
@@ -853,7 +853,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1728.285742712168</v>
+        <v>1789.77180773588</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>2292.857854367965</v>
+        <v>2317.614649165451</v>
       </c>
     </row>
     <row r="5">
@@ -869,7 +869,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>3022.014144835143</v>
+        <v>3108.410306271269</v>
       </c>
     </row>
     <row r="6">
@@ -877,7 +877,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>3970.844176971362</v>
+        <v>4132.305091068081</v>
       </c>
     </row>
     <row r="7">
@@ -885,7 +885,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>5120.698435794835</v>
+        <v>5295.178197064989</v>
       </c>
     </row>
     <row r="8">
@@ -893,7 +893,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>6275.546487038782</v>
+        <v>6350.082754054949</v>
       </c>
     </row>
     <row r="9">
@@ -901,7 +901,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>7801.026650989696</v>
+        <v>7819.997608619689</v>
       </c>
     </row>
     <row r="10">
@@ -909,7 +909,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>9224.317300905135</v>
+        <v>9262.444196831215</v>
       </c>
     </row>
     <row r="11">
@@ -917,7 +917,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>10642.39031562669</v>
+        <v>10708.63658873511</v>
       </c>
     </row>
     <row r="12">
@@ -925,7 +925,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>12060.8830247035</v>
+        <v>12159.62040651018</v>
       </c>
     </row>
     <row r="13">
@@ -933,7 +933,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>13475.9649576049</v>
+        <v>13610.06957485048</v>
       </c>
     </row>
     <row r="14">
@@ -941,7 +941,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>14891.0718144499</v>
+        <v>15063.41532861543</v>
       </c>
     </row>
     <row r="15">
@@ -949,7 +949,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>16306.1786712949</v>
+        <v>16513.37322415364</v>
       </c>
     </row>
     <row r="16">
@@ -957,7 +957,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>17725.78312445612</v>
+        <v>17958.97134747294</v>
       </c>
     </row>
     <row r="17">
@@ -965,7 +965,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>19262.37738258394</v>
+        <v>19608.25131226893</v>
       </c>
     </row>
     <row r="18">
@@ -973,7 +973,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>20253.37883959044</v>
+        <v>20615.72670305235</v>
       </c>
     </row>
     <row r="19">
@@ -981,7 +981,7 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>20851.33105802048</v>
+        <v>21205.80315066649</v>
       </c>
     </row>
     <row r="20">
@@ -989,7 +989,7 @@
         <v>2049</v>
       </c>
       <c r="B20" t="n">
-        <v>21426.08359133127</v>
+        <v>21797.15901440689</v>
       </c>
     </row>
     <row r="21">
@@ -997,7 +997,7 @@
         <v>2050</v>
       </c>
       <c r="B21" t="n">
-        <v>21991.09907120743</v>
+        <v>22380.67165662052</v>
       </c>
     </row>
     <row r="22">
@@ -1005,7 +1005,7 @@
         <v>2051</v>
       </c>
       <c r="B22" t="n">
-        <v>22513.00053549116</v>
+        <v>22960.91938795787</v>
       </c>
     </row>
     <row r="23">
@@ -1013,7 +1013,7 @@
         <v>2052</v>
       </c>
       <c r="B23" t="n">
-        <v>23033.43023255814</v>
+        <v>23564.77257016452</v>
       </c>
     </row>
     <row r="24">
@@ -1021,7 +1021,7 @@
         <v>2053</v>
       </c>
       <c r="B24" t="n">
-        <v>23544.12790697674</v>
+        <v>24167.35050783615</v>
       </c>
     </row>
     <row r="25">
@@ -1029,15 +1029,7 @@
         <v>2054</v>
       </c>
       <c r="B25" t="n">
-        <v>24053.51423746579</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2055</v>
-      </c>
-      <c r="B26" t="n">
-        <v>24563.61730623653</v>
+        <v>24756.57496468689</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1068,7 @@
         <v>2032</v>
       </c>
       <c r="B2" t="n">
-        <v>2100.788090051517</v>
+        <v>1992.536905323735</v>
       </c>
     </row>
     <row r="3">
@@ -1084,7 +1076,7 @@
         <v>2033</v>
       </c>
       <c r="B3" t="n">
-        <v>3360.693045196571</v>
+        <v>3111.416267637318</v>
       </c>
     </row>
     <row r="4">
@@ -1092,7 +1084,7 @@
         <v>2034</v>
       </c>
       <c r="B4" t="n">
-        <v>4621.066176147867</v>
+        <v>4336.207263445299</v>
       </c>
     </row>
     <row r="5">
@@ -1100,7 +1092,7 @@
         <v>2035</v>
       </c>
       <c r="B5" t="n">
-        <v>5814.115419579782</v>
+        <v>5567.884476013608</v>
       </c>
     </row>
     <row r="6">
@@ -1108,7 +1100,7 @@
         <v>2036</v>
       </c>
       <c r="B6" t="n">
-        <v>7025.568864549034</v>
+        <v>6708.001298602515</v>
       </c>
     </row>
     <row r="7">
@@ -1116,7 +1108,7 @@
         <v>2037</v>
       </c>
       <c r="B7" t="n">
-        <v>8245.456508266017</v>
+        <v>7952.911249180831</v>
       </c>
     </row>
     <row r="8">
@@ -1124,7 +1116,7 @@
         <v>2038</v>
       </c>
       <c r="B8" t="n">
-        <v>9462.154934163585</v>
+        <v>9255.80789060182</v>
       </c>
     </row>
     <row r="9">
@@ -1132,7 +1124,7 @@
         <v>2039</v>
       </c>
       <c r="B9" t="n">
-        <v>11293.72622110342</v>
+        <v>11287.71256951713</v>
       </c>
     </row>
     <row r="10">
@@ -1140,7 +1132,7 @@
         <v>2040</v>
       </c>
       <c r="B10" t="n">
-        <v>13184.73675914425</v>
+        <v>13311.98782436536</v>
       </c>
     </row>
     <row r="11">
@@ -1148,7 +1140,7 @@
         <v>2041</v>
       </c>
       <c r="B11" t="n">
-        <v>15316.19694713837</v>
+        <v>15449.02604170104</v>
       </c>
     </row>
     <row r="12">
@@ -1156,7 +1148,7 @@
         <v>2042</v>
       </c>
       <c r="B12" t="n">
-        <v>17493.03617798383</v>
+        <v>17651.19698277635</v>
       </c>
     </row>
     <row r="13">
@@ -1164,7 +1156,7 @@
         <v>2043</v>
       </c>
       <c r="B13" t="n">
-        <v>19750.51157410862</v>
+        <v>19753.28364129357</v>
       </c>
     </row>
     <row r="14">
@@ -1172,7 +1164,7 @@
         <v>2044</v>
       </c>
       <c r="B14" t="n">
-        <v>21445.47684804241</v>
+        <v>21267.92801500317</v>
       </c>
     </row>
     <row r="15">
@@ -1180,7 +1172,7 @@
         <v>2045</v>
       </c>
       <c r="B15" t="n">
-        <v>22869.62190811221</v>
+        <v>22340.31378137568</v>
       </c>
     </row>
     <row r="16">
@@ -1188,7 +1180,7 @@
         <v>2046</v>
       </c>
       <c r="B16" t="n">
-        <v>23910.76788544547</v>
+        <v>23376.62374306103</v>
       </c>
     </row>
     <row r="17">
@@ -1196,7 +1188,7 @@
         <v>2047</v>
       </c>
       <c r="B17" t="n">
-        <v>25071.64293968679</v>
+        <v>24556.33076731603</v>
       </c>
     </row>
     <row r="18">
@@ -1204,7 +1196,7 @@
         <v>2048</v>
       </c>
       <c r="B18" t="n">
-        <v>26065.49263538764</v>
+        <v>25551.27324557401</v>
       </c>
     </row>
     <row r="19">
@@ -1212,7 +1204,7 @@
         <v>2049</v>
       </c>
       <c r="B19" t="n">
-        <v>27049.25545867653</v>
+        <v>26541.54169241404</v>
       </c>
     </row>
     <row r="20">
@@ -1220,7 +1212,7 @@
         <v>2050</v>
       </c>
       <c r="B20" t="n">
-        <v>28038.76765767459</v>
+        <v>27531.30099946307</v>
       </c>
     </row>
     <row r="21">
@@ -1228,7 +1220,7 @@
         <v>2051</v>
       </c>
       <c r="B21" t="n">
-        <v>29030.47256176306</v>
+        <v>28553.29271574779</v>
       </c>
     </row>
     <row r="22">
@@ -1236,7 +1228,7 @@
         <v>2052</v>
       </c>
       <c r="B22" t="n">
-        <v>30105.18084692169</v>
+        <v>29609.45417951032</v>
       </c>
     </row>
     <row r="23">
@@ -1244,7 +1236,7 @@
         <v>2053</v>
       </c>
       <c r="B23" t="n">
-        <v>31159.64732010838</v>
+        <v>30778.7998683004</v>
       </c>
     </row>
     <row r="24">
@@ -1252,7 +1244,7 @@
         <v>2054</v>
       </c>
       <c r="B24" t="n">
-        <v>32116.49740373248</v>
+        <v>31841.76789504404</v>
       </c>
     </row>
     <row r="25">
@@ -1260,7 +1252,7 @@
         <v>2055</v>
       </c>
       <c r="B25" t="n">
-        <v>33075.58070431934</v>
+        <v>32937.34591886247</v>
       </c>
     </row>
     <row r="26">
@@ -1268,7 +1260,7 @@
         <v>2056</v>
       </c>
       <c r="B26" t="n">
-        <v>34142.16066517226</v>
+        <v>34177.53899456122</v>
       </c>
     </row>
   </sheetData>
@@ -1282,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1307,7 +1299,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>1020.793950850662</v>
+        <v>1106.975238711766</v>
       </c>
     </row>
     <row r="3">
@@ -1315,7 +1307,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>2039.232331818461</v>
+        <v>2104.378549308913</v>
       </c>
     </row>
     <row r="4">
@@ -1323,7 +1315,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>3432.983475196653</v>
+        <v>3463.895201846325</v>
       </c>
     </row>
     <row r="5">
@@ -1331,7 +1323,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>4985.631588892019</v>
+        <v>5095.566908218865</v>
       </c>
     </row>
     <row r="6">
@@ -1339,7 +1331,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>6752.393779772964</v>
+        <v>6968.925701767374</v>
       </c>
     </row>
     <row r="7">
@@ -1347,7 +1339,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>8708.089550481423</v>
+        <v>8969.653240774353</v>
       </c>
     </row>
     <row r="8">
@@ -1355,7 +1347,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>10660.21609948145</v>
+        <v>10856.96648750686</v>
       </c>
     </row>
     <row r="9">
@@ -1363,7 +1355,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>12575.1801344746</v>
+        <v>12814.49945473534</v>
       </c>
     </row>
     <row r="10">
@@ -1371,7 +1363,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>15022.8644588079</v>
+        <v>15507.38722164896</v>
       </c>
     </row>
     <row r="11">
@@ -1379,7 +1371,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>17481.99944329268</v>
+        <v>18172.49265951406</v>
       </c>
     </row>
     <row r="12">
@@ -1387,7 +1379,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>19993.11046734116</v>
+        <v>20821.34877787585</v>
       </c>
     </row>
     <row r="13">
@@ -1395,7 +1387,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>22540.30641915152</v>
+        <v>23446.01547704969</v>
       </c>
     </row>
     <row r="14">
@@ -1403,7 +1395,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>25184.70384606915</v>
+        <v>25967.79259285823</v>
       </c>
     </row>
     <row r="15">
@@ -1411,7 +1403,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>27424.41408537074</v>
+        <v>27968.67806990608</v>
       </c>
     </row>
     <row r="16">
@@ -1419,7 +1411,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>29402.66073679991</v>
+        <v>29450.36582451781</v>
       </c>
     </row>
     <row r="17">
@@ -1427,7 +1419,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>31009.5540103765</v>
+        <v>31139.41455231239</v>
       </c>
     </row>
     <row r="18">
@@ -1435,7 +1427,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>31993.94343501695</v>
+        <v>32045.5110107284</v>
       </c>
     </row>
     <row r="19">
@@ -1443,7 +1435,7 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>32489.42068341254</v>
+        <v>32540.14680971203</v>
       </c>
     </row>
     <row r="20">
@@ -1451,7 +1443,7 @@
         <v>2049</v>
       </c>
       <c r="B20" t="n">
-        <v>32986.36569359584</v>
+        <v>33036.5296803653</v>
       </c>
     </row>
     <row r="21">
@@ -1459,7 +1451,7 @@
         <v>2050</v>
       </c>
       <c r="B21" t="n">
-        <v>33486.27204749129</v>
+        <v>33536.5296803653</v>
       </c>
     </row>
     <row r="22">
@@ -1467,7 +1459,7 @@
         <v>2051</v>
       </c>
       <c r="B22" t="n">
-        <v>33986.3005879331</v>
+        <v>34036.5296803653</v>
       </c>
     </row>
     <row r="23">
@@ -1475,15 +1467,7 @@
         <v>2052</v>
       </c>
       <c r="B23" t="n">
-        <v>34486.30136986302</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>2053</v>
-      </c>
-      <c r="B24" t="n">
-        <v>34987.67123287671</v>
+        <v>34536.5296803653</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +1481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,7 +1506,7 @@
         <v>2031</v>
       </c>
       <c r="B2" t="n">
-        <v>1020.793950850662</v>
+        <v>1106.975238711766</v>
       </c>
     </row>
     <row r="3">
@@ -1530,7 +1514,7 @@
         <v>2032</v>
       </c>
       <c r="B3" t="n">
-        <v>1728.285742712168</v>
+        <v>1789.77180773588</v>
       </c>
     </row>
     <row r="4">
@@ -1538,7 +1522,7 @@
         <v>2033</v>
       </c>
       <c r="B4" t="n">
-        <v>3476.842044841405</v>
+        <v>3495.535124433279</v>
       </c>
     </row>
     <row r="5">
@@ -1546,7 +1530,7 @@
         <v>2034</v>
       </c>
       <c r="B5" t="n">
-        <v>5386.747596299856</v>
+        <v>5461.032894852641</v>
       </c>
     </row>
     <row r="6">
@@ -1554,7 +1538,7 @@
         <v>2035</v>
       </c>
       <c r="B6" t="n">
-        <v>7519.306667389053</v>
+        <v>7665.663761242734</v>
       </c>
     </row>
     <row r="7">
@@ -1562,7 +1546,7 @@
         <v>2036</v>
       </c>
       <c r="B7" t="n">
-        <v>10294.99149913791</v>
+        <v>10457.45146654837</v>
       </c>
     </row>
     <row r="8">
@@ -1570,7 +1554,7 @@
         <v>2037</v>
       </c>
       <c r="B8" t="n">
-        <v>13171.92358050162</v>
+        <v>13236.7149592529</v>
       </c>
     </row>
     <row r="9">
@@ -1578,7 +1562,7 @@
         <v>2038</v>
       </c>
       <c r="B9" t="n">
-        <v>16228.91888841308</v>
+        <v>16239.80859929818</v>
       </c>
     </row>
     <row r="10">
@@ -1586,7 +1570,7 @@
         <v>2039</v>
       </c>
       <c r="B10" t="n">
-        <v>19647.12292875741</v>
+        <v>19760.73244453446</v>
       </c>
     </row>
     <row r="11">
@@ -1594,7 +1578,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>23442.09353861278</v>
+        <v>23717.76752940902</v>
       </c>
     </row>
     <row r="12">
@@ -1602,7 +1586,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>27634.67222762048</v>
+        <v>27863.67516887463</v>
       </c>
     </row>
     <row r="13">
@@ -1610,7 +1594,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>32200.56862013246</v>
+        <v>32303.26250546046</v>
       </c>
     </row>
     <row r="14">
@@ -1618,7 +1602,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>36705.95236495582</v>
+        <v>36814.00426987503</v>
       </c>
     </row>
     <row r="15">
@@ -1626,7 +1610,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>41219.71149603026</v>
+        <v>41329.17008787573</v>
       </c>
     </row>
     <row r="16">
@@ -1634,7 +1618,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>45680.72201222426</v>
+        <v>45583.5963688373</v>
       </c>
     </row>
     <row r="17">
@@ -1642,7 +1626,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>49634.36145522023</v>
+        <v>49660.04491817566</v>
       </c>
     </row>
     <row r="18">
@@ -1650,7 +1634,7 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>52918.53384826249</v>
+        <v>52536.26117655997</v>
       </c>
     </row>
     <row r="19">
@@ -1658,7 +1642,15 @@
         <v>2048</v>
       </c>
       <c r="B19" t="n">
-        <v>54632.89608898023</v>
+        <v>54058.62054410805</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B20" t="n">
+        <v>54696.65732959851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update deployment plot labels
</commit_message>
<xml_diff>
--- a/analysis/results/cumulative-capacity.xlsx
+++ b/analysis/results/cumulative-capacity.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +522,7 @@
         <v>2040</v>
       </c>
       <c r="B11" t="n">
-        <v>26449.3016289559</v>
+        <v>26541.71939820418</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>2041</v>
       </c>
       <c r="B12" t="n">
-        <v>30345.01003930124</v>
+        <v>31180.7898679445</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>2042</v>
       </c>
       <c r="B13" t="n">
-        <v>34514.95913616559</v>
+        <v>35927.35275193814</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>2043</v>
       </c>
       <c r="B14" t="n">
-        <v>38342.47413945558</v>
+        <v>40590.58779680728</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>2044</v>
       </c>
       <c r="B15" t="n">
-        <v>42226.14206020704</v>
+        <v>45096.14405351903</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>2045</v>
       </c>
       <c r="B16" t="n">
-        <v>46159.60327859426</v>
+        <v>49796.00380965499</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>2046</v>
       </c>
       <c r="B17" t="n">
-        <v>50046.98899521399</v>
+        <v>53747.17892691874</v>
       </c>
     </row>
     <row r="18">
@@ -578,14 +578,6 @@
         <v>2047</v>
       </c>
       <c r="B18" t="n">
-        <v>53593.00354607464</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2048</v>
-      </c>
-      <c r="B19" t="n">
         <v>54601.2927938712</v>
       </c>
     </row>

</xml_diff>